<commit_message>
good spoon and peach
</commit_message>
<xml_diff>
--- a/Dataset/Parameters Configuration.xlsx
+++ b/Dataset/Parameters Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unigeit-my.sharepoint.com/personal/christian_gianoglio_unige_it/Documents/Università/Cosmic/Cosmic GitHub/Force_recontruction_algorithm/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="11_F25DC773A252ABDACC1048E6419842F25BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA8C7D03-46B1-46C8-8163-3614E32F1A82}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="11_F25DC773A252ABDACC1048E6419842F25BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C4D449B-9B07-43AC-BA60-977F621BC973}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>NW</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>28 no release</t>
-  </si>
-  <si>
-    <t>5 e 26</t>
   </si>
   <si>
     <t>13,17,18</t>
@@ -449,7 +446,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,17 +509,17 @@
       <c r="D2" s="3">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G2" s="1">
         <v>50</v>
       </c>
       <c r="H2" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I2" s="1">
         <v>500</v>
@@ -530,9 +527,7 @@
       <c r="J2" s="1">
         <v>10</v>
       </c>
-      <c r="K2" s="5">
-        <v>18</v>
-      </c>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -547,17 +542,17 @@
       <c r="D3" s="3">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G3" s="1">
         <v>50</v>
       </c>
       <c r="H3" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1">
         <v>500</v>
@@ -580,17 +575,17 @@
       <c r="D4" s="3">
         <v>10</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G4" s="1">
         <v>50</v>
       </c>
       <c r="H4" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I4" s="1">
         <v>500</v>
@@ -615,17 +610,17 @@
       <c r="D5" s="3">
         <v>10</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G5" s="1">
         <v>50</v>
       </c>
       <c r="H5" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I5" s="1">
         <v>500</v>
@@ -633,9 +628,7 @@
       <c r="J5" s="1">
         <v>10</v>
       </c>
-      <c r="K5" s="6">
-        <v>26</v>
-      </c>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -650,17 +643,17 @@
       <c r="D6" s="3">
         <v>10</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G6" s="1">
         <v>50</v>
       </c>
       <c r="H6" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I6" s="1">
         <v>500</v>
@@ -683,17 +676,17 @@
       <c r="D7" s="3">
         <v>10</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G7" s="1">
         <v>50</v>
       </c>
       <c r="H7" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I7" s="1">
         <v>500</v>
@@ -718,17 +711,17 @@
       <c r="D8" s="3">
         <v>10</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>1</v>
       </c>
       <c r="F8" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G8" s="1">
         <v>50</v>
       </c>
       <c r="H8" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I8" s="1">
         <v>500</v>
@@ -736,8 +729,8 @@
       <c r="J8" s="3">
         <v>10</v>
       </c>
-      <c r="K8" s="6" t="s">
-        <v>11</v>
+      <c r="K8" s="6">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +744,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,17 +807,17 @@
       <c r="D2" s="3">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>0.05</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>0.3</v>
       </c>
       <c r="G2" s="1">
         <v>50</v>
       </c>
-      <c r="H2" s="1">
-        <v>5</v>
+      <c r="H2" s="3">
+        <v>10</v>
       </c>
       <c r="I2" s="1">
         <v>500</v>
@@ -847,17 +840,17 @@
       <c r="D3" s="3">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>0.05</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>0.3</v>
       </c>
       <c r="G3" s="1">
         <v>50</v>
       </c>
-      <c r="H3" s="1">
-        <v>5</v>
+      <c r="H3" s="3">
+        <v>10</v>
       </c>
       <c r="I3" s="1">
         <v>500</v>
@@ -865,9 +858,7 @@
       <c r="J3" s="1">
         <v>10</v>
       </c>
-      <c r="K3" s="6">
-        <v>5</v>
-      </c>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -882,17 +873,17 @@
       <c r="D4" s="3">
         <v>10</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="2">
         <v>0.05</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>0.3</v>
       </c>
       <c r="G4" s="1">
         <v>50</v>
       </c>
-      <c r="H4" s="1">
-        <v>5</v>
+      <c r="H4" s="3">
+        <v>10</v>
       </c>
       <c r="I4" s="1">
         <v>500</v>
@@ -915,17 +906,17 @@
       <c r="D5" s="3">
         <v>10</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>0.05</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>0.3</v>
       </c>
       <c r="G5" s="1">
         <v>50</v>
       </c>
-      <c r="H5" s="1">
-        <v>5</v>
+      <c r="H5" s="3">
+        <v>10</v>
       </c>
       <c r="I5" s="1">
         <v>500</v>
@@ -950,17 +941,17 @@
       <c r="D6" s="3">
         <v>10</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>0.05</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>0.3</v>
       </c>
       <c r="G6" s="1">
         <v>50</v>
       </c>
-      <c r="H6" s="1">
-        <v>5</v>
+      <c r="H6" s="3">
+        <v>10</v>
       </c>
       <c r="I6" s="1">
         <v>500</v>
@@ -983,17 +974,17 @@
       <c r="D7" s="3">
         <v>10</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>0.05</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>0.3</v>
       </c>
       <c r="G7" s="1">
         <v>50</v>
       </c>
-      <c r="H7" s="1">
-        <v>5</v>
+      <c r="H7" s="3">
+        <v>10</v>
       </c>
       <c r="I7" s="1">
         <v>500</v>
@@ -1018,17 +1009,17 @@
       <c r="D8" s="3">
         <v>10</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>0.05</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <v>0.3</v>
       </c>
       <c r="G8" s="1">
         <v>50</v>
       </c>
-      <c r="H8" s="1">
-        <v>5</v>
+      <c r="H8" s="3">
+        <v>10</v>
       </c>
       <c r="I8" s="1">
         <v>500</v>
@@ -1120,7 +1111,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>